<commit_message>
Open loop with graphs
</commit_message>
<xml_diff>
--- a/Lab 3/Data.xlsx
+++ b/Lab 3/Data.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melab2\Desktop\Mechanical-Control-Systems\Lab 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Documents\GitHub\Mechanical Control Systems\Lab 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5193A69-424D-4478-84B8-AEBB94074E19}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="2"/>
+    <workbookView minimized="1" xWindow="1104" yWindow="2820" windowWidth="17280" windowHeight="9024" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 - Valve" sheetId="2" r:id="rId1"/>
     <sheet name="Part 2 - Pressure Transducer" sheetId="1" r:id="rId2"/>
     <sheet name="Step Response" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Bottom Tank Height (in)</t>
   </si>
@@ -66,11 +73,29 @@
   <si>
     <t>DISTURBANCE</t>
   </si>
+  <si>
+    <t>Top Tank 1Tau Height (in)</t>
+  </si>
+  <si>
+    <t>Top Tank Tau (s)</t>
+  </si>
+  <si>
+    <t>Qi2/H1 Gain</t>
+  </si>
+  <si>
+    <t>Bottom Tank "1Tau" Height (in)</t>
+  </si>
+  <si>
+    <t>Bottom Tank "Tau" (s)</t>
+  </si>
+  <si>
+    <t>TopHeight/GPM Gain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -842,7 +867,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -920,7 +944,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1273,7 +1296,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1351,7 +1373,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1704,7 +1725,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1782,7 +1802,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2117,7 +2136,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Bottom Tank Height vs. Vhbttm Linear</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2195,7 +2238,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5868,7 +5910,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5900,7 +5948,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5937,7 +5991,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5969,7 +6029,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6001,7 +6067,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6033,7 +6105,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -6315,20 +6393,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -6342,7 +6420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -6356,7 +6434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -6370,7 +6448,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5.5</v>
       </c>
@@ -6384,7 +6462,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -6398,7 +6476,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -6419,22 +6497,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A21" sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6448,7 +6526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -6459,7 +6537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19</v>
       </c>
@@ -6470,7 +6548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>18</v>
       </c>
@@ -6481,7 +6559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>17</v>
       </c>
@@ -6492,7 +6570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -6506,7 +6584,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -6520,7 +6598,7 @@
         <v>3.53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>14</v>
       </c>
@@ -6534,7 +6612,7 @@
         <v>3.8620000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>13</v>
       </c>
@@ -6548,7 +6626,7 @@
         <v>4.2290000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12</v>
       </c>
@@ -6562,7 +6640,7 @@
         <v>4.6040000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -6576,7 +6654,7 @@
         <v>4.9710000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -6590,7 +6668,7 @@
         <v>5.3659999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -6604,7 +6682,7 @@
         <v>5.742</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -6618,7 +6696,7 @@
         <v>6.1230000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -6632,7 +6710,7 @@
         <v>6.4889999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>6</v>
       </c>
@@ -6646,7 +6724,7 @@
         <v>6.8650000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -6660,7 +6738,7 @@
         <v>7.2169999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -6674,7 +6752,7 @@
         <v>7.6120000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -6685,7 +6763,7 @@
         <v>7.9829999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -6696,7 +6774,7 @@
         <v>8.1449999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -6707,7 +6785,7 @@
         <v>8.2669999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -6726,19 +6804,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="25.7109375" customWidth="1"/>
+    <col min="1" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="6" width="25.77734375" customWidth="1"/>
+    <col min="7" max="10" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -6748,40 +6828,95 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
         <v>3.5</v>
       </c>
+      <c r="C3">
+        <v>7.25</v>
+      </c>
       <c r="D3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4">
         <v>3.75</v>
       </c>
+      <c r="C4">
+        <v>9.25</v>
+      </c>
+      <c r="D4">
+        <v>7.5</v>
+      </c>
+      <c r="E4">
+        <f>C3+0.632*(C4-C3)</f>
+        <v>8.5139999999999993</v>
+      </c>
+      <c r="F4">
+        <f>D3+0.632*(D4-D3)</f>
+        <v>6.9480000000000004</v>
+      </c>
+      <c r="G4">
+        <v>88</v>
+      </c>
+      <c r="H4">
+        <v>163</v>
+      </c>
+      <c r="I4">
+        <f>(C4-C3)/(((B4*10.399-6.1525)*0.062+0.15)-((B3*10.399-6.1525)*0.062+0.15))</f>
+        <v>12.408140981297791</v>
+      </c>
+      <c r="J4">
+        <f>((B4*10.399-6.1525)*0.062+0.15)/C4</f>
+        <v>0.23635810810810812</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>3.75</v>
       </c>
+      <c r="C6">
+        <v>9.25</v>
+      </c>
+      <c r="D6">
+        <v>7.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -6791,8 +6926,33 @@
       <c r="C7">
         <v>11.5</v>
       </c>
+      <c r="D7">
+        <v>9.5</v>
+      </c>
+      <c r="E7">
+        <f>C6+0.632*(C7-C6)</f>
+        <v>10.672000000000001</v>
+      </c>
+      <c r="F7">
+        <f>D6+0.632*(D7-D6)</f>
+        <v>8.7639999999999993</v>
+      </c>
+      <c r="G7">
+        <v>105</v>
+      </c>
+      <c r="H7">
+        <v>169</v>
+      </c>
+      <c r="I7">
+        <f>(C7-C6)/(((B7*10.399-6.1525)*0.062+0.15)-((B6*10.399-6.1525)*0.062+0.15))</f>
+        <v>13.959158603960091</v>
+      </c>
+      <c r="J7">
+        <f>((B7*10.399-6.1525)*0.062+0.15)/C7</f>
+        <v>0.20413017391304344</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6802,8 +6962,11 @@
       <c r="C9">
         <v>11.5</v>
       </c>
+      <c r="D9">
+        <v>9.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6816,13 +6979,45 @@
       <c r="D10">
         <v>11.25</v>
       </c>
+      <c r="E10">
+        <f>C9+0.632*(C10-C9)</f>
+        <v>13.08</v>
+      </c>
+      <c r="F10">
+        <f>D9+0.632*(D10-D9)</f>
+        <v>10.606</v>
+      </c>
+      <c r="G10">
+        <v>109</v>
+      </c>
+      <c r="H10">
+        <v>192</v>
+      </c>
+      <c r="I10">
+        <f>(C10-C9)/(((B10*10.399-6.1525)*0.062+0.15)-((B9*10.399-6.1525)*0.062+0.15))</f>
+        <v>15.510176226622281</v>
+      </c>
+      <c r="J10">
+        <f>((B10*10.399-6.1525)*0.062+0.15)/C10</f>
+        <v>0.1791915357142857</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <f>AVERAGE(I4,I7,I10)</f>
+        <v>13.959158603960054</v>
+      </c>
+      <c r="J13">
+        <f>AVERAGE(J4,J7,J10)</f>
+        <v>0.20655993924514574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -6836,7 +7031,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -6848,6 +7043,14 @@
       </c>
       <c r="D16">
         <v>7.25</v>
+      </c>
+      <c r="E16">
+        <f>C15+0.632*(C16-C15)</f>
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <f>D15+0.632*(D16-D15)</f>
+        <v>8.7219999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished collecting experimental data
</commit_message>
<xml_diff>
--- a/Lab 3/Data.xlsx
+++ b/Lab 3/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="2820" windowWidth="17280" windowHeight="9030" activeTab="3"/>
+    <workbookView xWindow="1110" yWindow="2820" windowWidth="17280" windowHeight="9030" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 - Valve" sheetId="2" r:id="rId1"/>
@@ -125,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,12 +133,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,7 +181,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -249,7 +258,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -530,7 +538,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -608,7 +615,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -883,7 +889,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -961,7 +966,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1314,7 +1318,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1392,7 +1395,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1745,7 +1747,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1823,7 +1824,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2183,7 +2183,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2261,7 +2260,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6831,8 +6829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7035,8 +7033,8 @@
         <v>0.20655993924514574</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -7085,7 +7083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>